<commit_message>
Added enclosure, removed unnecessary resistor
</commit_message>
<xml_diff>
--- a/Servo_Controller/Docs/Manufacturing data/JLCSMT_BOM.xlsx
+++ b/Servo_Controller/Docs/Manufacturing data/JLCSMT_BOM.xlsx
@@ -210,7 +210,7 @@
     <t xml:space="preserve">4.7k</t>
   </si>
   <si>
-    <t xml:space="preserve">R1,R2,R3</t>
+    <t xml:space="preserve">R2,R3</t>
   </si>
   <si>
     <t xml:space="preserve">C304616</t>
@@ -569,7 +569,7 @@
   <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8828125" defaultRowHeight="20" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>